<commit_message>
Update .xlsx new branch
</commit_message>
<xml_diff>
--- a/Libro1.xlsx
+++ b/Libro1.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Primero</t>
   </si>
@@ -40,6 +41,9 @@
   </si>
   <si>
     <t>gate</t>
+  </si>
+  <si>
+    <t>hide</t>
   </si>
 </sst>
 </file>
@@ -388,6 +392,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
@@ -396,7 +420,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New sheet in a .xlsx file
</commit_message>
<xml_diff>
--- a/Libro1.xlsx
+++ b/Libro1.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
+    <sheet name="Hoja4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Primero</t>
   </si>
@@ -44,6 +45,9 @@
   </si>
   <si>
     <t>hide</t>
+  </si>
+  <si>
+    <t>otherside</t>
   </si>
 </sst>
 </file>
@@ -412,6 +416,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
@@ -420,7 +444,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update sheet in .xlsx file
</commit_message>
<xml_diff>
--- a/Libro1.xlsx
+++ b/Libro1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Primero</t>
   </si>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t>otherside</t>
+  </si>
+  <si>
+    <t>SuperHide</t>
   </si>
 </sst>
 </file>
@@ -414,6 +417,29 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -424,26 +450,6 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update again sheet .xlsx file
</commit_message>
<xml_diff>
--- a/Libro1.xlsx
+++ b/Libro1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Primero</t>
   </si>
@@ -41,9 +41,6 @@
     <t>qUINTA</t>
   </si>
   <si>
-    <t>gate</t>
-  </si>
-  <si>
     <t>hide</t>
   </si>
   <si>
@@ -51,6 +48,12 @@
   </si>
   <si>
     <t>SuperHide</t>
+  </si>
+  <si>
+    <t>call</t>
+  </si>
+  <si>
+    <t>gateway</t>
   </si>
 </sst>
 </file>
@@ -397,17 +400,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -419,7 +425,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -427,10 +433,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -450,7 +456,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>